<commit_message>
Se agrega el grafico de las derivadas discretas
</commit_message>
<xml_diff>
--- a/cruces.xlsx
+++ b/cruces.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2003-02-04</t>
+          <t>2005-03-22</t>
         </is>
       </c>
     </row>
@@ -457,7 +457,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2003-02-19</t>
+          <t>2005-03-30</t>
         </is>
       </c>
     </row>
@@ -467,7 +467,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2003-02-21</t>
+          <t>2005-03-31</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2003-04-24</t>
+          <t>2005-11-02</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2003-04-25</t>
+          <t>2005-11-16</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2003-05-01</t>
+          <t>2006-01-09</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2003-05-07</t>
+          <t>2006-01-10</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2003-06-06</t>
+          <t>2006-01-11</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2003-06-09</t>
+          <t>2006-01-20</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2003-06-12</t>
+          <t>2006-01-23</t>
         </is>
       </c>
     </row>
@@ -547,187 +547,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2003-06-13</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2003-07-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2003-07-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2003-07-14</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>2005-04-08</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>2005-04-22</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2005-04-25</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>2005-04-27</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>2006-06-08</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>2006-07-27</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>2006-08-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2006-08-11</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>2007-02-28</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>2007-03-01</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>2007-07-24</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>2007-08-27</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>2007-08-29</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>2007-09-05</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>2007-09-07</t>
+          <t>2006-01-24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios para usar el nuevo path
</commit_message>
<xml_diff>
--- a/cruces.xlsx
+++ b/cruces.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="B1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,116 +441,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2005-03-22</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2005-03-30</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2005-03-31</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2005-11-02</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2005-11-16</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2006-01-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2006-01-10</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2006-01-11</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2006-01-20</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2006-01-23</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2006-01-24</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>